<commit_message>
Finished the Correlation of Determination equation in spike solution!! Very rough but a good guide.
</commit_message>
<xml_diff>
--- a/correlation.xlsx
+++ b/correlation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\backe\OD\2019\BCPR280 - Software Engineering 2\A. Assessments\Assignment 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bea82\OneDrive - Ara Institute of Canterbury\2019\BCPR280 - Software Engineering 2\A. Assessments\Assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_A4E4DD86F162D0725F6F86713C839A7FDCFB8BA6" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{21A7540D-997E-40BA-9426-615A78DB209E}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_A4E4DD86F162D0725F6F86713C839A7FDCFB8BA6" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EC89896F-F21A-4A9A-A445-589347BDD937}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="630" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,9 +216,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>393700</xdr:colOff>
+          <xdr:colOff>390525</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>107950</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -270,9 +270,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>260350</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>69850</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -378,7 +378,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>374650</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -432,9 +432,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>298450</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -486,9 +486,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>165100</xdr:colOff>
+          <xdr:colOff>161925</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -795,18 +795,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H28"/>
+  <dimension ref="A2:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="7" width="10.81640625" customWidth="1"/>
+    <col min="3" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
@@ -823,7 +823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -850,7 +850,7 @@
         <v>929.59999999999991</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -873,7 +873,7 @@
         <v>86.490000000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -896,7 +896,7 @@
         <v>466.56000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -919,7 +919,7 @@
         <v>47.610000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f>COUNT(B3:B7)</f>
         <v>5</v>
@@ -946,7 +946,7 @@
         <v>104.03999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="6">
         <f>SUM(C3:C7)</f>
         <v>580</v>
@@ -967,8 +967,18 @@
         <f t="shared" si="1"/>
         <v>830.14</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" s="6">
+        <f>SUM(sum_x*sum_y)</f>
+        <v>34336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f>SUM(5*74498)</f>
+        <v>372490</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="6">
         <f>n</f>
         <v>5</v>
@@ -986,7 +996,7 @@
         <v>59.2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="6">
         <f>n</f>
         <v>5</v>
@@ -1012,7 +1022,7 @@
         <v>59.2</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17">
         <f>C12*D12</f>
         <v>38738.5</v>
@@ -1022,7 +1032,7 @@
         <v>34336</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>(C13*D13)-(E13*E13)</f>
         <v>36090</v>
@@ -1032,37 +1042,51 @@
         <v>646.05999999999949</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D20">
         <f>C17-E17</f>
         <v>4402.5</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="M20">
+        <f>SUM(5*74498)</f>
+        <v>372490</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D21">
         <f>C18*E18</f>
         <v>23316305.39999998</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="M21">
+        <f>SUM(580*580)</f>
+        <v>336400</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <f>M20-M21</f>
+        <v>36090</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D23">
         <f>D20</f>
         <v>4402.5</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D24">
         <f>SQRT(D21)</f>
         <v>4828.6960351631142</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D26" s="7">
         <f>D23/D24</f>
         <v>0.91173682665889377</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D28" s="7">
         <f>rxy*rxy</f>
         <v>0.83126404108602969</v>
@@ -1087,9 +1111,9 @@
               </from>
               <to>
                 <xdr:col>14</xdr:col>
-                <xdr:colOff>393700</xdr:colOff>
+                <xdr:colOff>390525</xdr:colOff>
                 <xdr:row>13</xdr:row>
-                <xdr:rowOff>107950</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1112,9 +1136,9 @@
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>260350</xdr:colOff>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>18</xdr:row>
-                <xdr:rowOff>69850</xdr:rowOff>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1162,7 +1186,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>374650</xdr:colOff>
+                <xdr:colOff>371475</xdr:colOff>
                 <xdr:row>26</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -1187,9 +1211,9 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>298450</xdr:colOff>
+                <xdr:colOff>295275</xdr:colOff>
                 <xdr:row>28</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1212,9 +1236,9 @@
               </from>
               <to>
                 <xdr:col>15</xdr:col>
-                <xdr:colOff>165100</xdr:colOff>
+                <xdr:colOff>161925</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>184150</xdr:rowOff>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>

</xml_diff>